<commit_message>
Comentado e Organizado pt.2
</commit_message>
<xml_diff>
--- a/Resultados/Material/ResNet/Tentativa 1.xlsx
+++ b/Resultados/Material/ResNet/Tentativa 1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr codeName="EsteLivro" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\beatr\Documents\GitHub\SAFENET-Bea\Resultados\Material\ResNet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CEEB61D-93ED-4951-9811-37E67F481A71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6673A34-A317-4FE4-AFB3-0FE48B8E8D0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{44EB1693-29A4-4AD6-9832-A8AEAD2DC94E}"/>
   </bookViews>
@@ -1550,14 +1550,14 @@
   <sheetPr codeName="Folha1"/>
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -1885,7 +1885,7 @@
   <dimension ref="N1:O44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2096,7 +2096,9 @@
   <sheetPr codeName="Folha2"/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R16" sqref="R16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
@@ -2110,7 +2112,9 @@
   <sheetPr codeName="Folha3"/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0"/>
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="S15" sqref="S15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
@@ -2125,7 +2129,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:F6"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2256,7 +2260,7 @@
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
+      <selection pane="bottomLeft" activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2264,15 +2268,16 @@
     <col min="1" max="1" width="8.6328125" style="28" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.6328125" style="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.453125" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.6328125" style="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.26953125" style="26" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.90625" style="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" style="26" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.54296875" customWidth="1"/>
     <col min="7" max="7" width="6.453125" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.81640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.1796875" style="9" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.7265625" style="9"/>
     <col min="10" max="10" width="3.81640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.6328125" style="19" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="4.36328125" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.6328125" style="19" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3.81640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.36328125" style="9" bestFit="1" customWidth="1"/>
     <col min="14" max="16384" width="8.7265625" style="9"/>
   </cols>
   <sheetData>
@@ -2531,25 +2536,25 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H8" sqref="H8"/>
+      <selection pane="topRight" activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.7265625" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.54296875" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.90625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.26953125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.54296875" style="33" customWidth="1"/>
     <col min="7" max="7" width="12.6328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.7265625" style="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="105.1796875" style="35" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.08984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.90625" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.08984375" style="35" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="36" t="s">
         <v>30</v>
       </c>
@@ -2582,7 +2587,7 @@
       </c>
       <c r="K1"/>
     </row>
-    <row r="2" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="15">
         <v>0</v>
       </c>
@@ -2620,7 +2625,7 @@
       </c>
       <c r="K2"/>
     </row>
-    <row r="3" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="15">
         <v>1</v>
       </c>
@@ -2658,7 +2663,7 @@
       </c>
       <c r="K3"/>
     </row>
-    <row r="4" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="15">
         <v>2</v>
       </c>
@@ -2696,7 +2701,7 @@
       </c>
       <c r="K4"/>
     </row>
-    <row r="5" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>8</v>
       </c>
@@ -2736,7 +2741,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
         <v>9</v>
       </c>
@@ -2776,7 +2781,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="11">
         <v>0</v>
       </c>
@@ -2816,7 +2821,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="11">
         <v>1</v>
       </c>
@@ -2856,7 +2861,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="12" t="s">
         <v>8</v>
       </c>
@@ -2896,7 +2901,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="13" t="s">
         <v>9</v>
       </c>
@@ -2937,7 +2942,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="11"/>
       <c r="G11">
         <f>SUM(G5:G10)+B7</f>

</xml_diff>